<commit_message>
03-01-2019 - 1st commit
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.achas\eclipse-workspace\simpleOrdering\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13060CEF-9654-461A-B1F6-1C6637EC2E75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21686C7-F29D-4F41-9328-4501A2C0210A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment_DirectSales" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="TC2" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -587,7 +586,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,7 +691,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798AD516-E464-4708-9D8E-52009CD3236C}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,7 +894,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B66D6326-C1D0-467D-8F1E-D5B4A578621C}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
06/01 - LA's First Commit
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.achas\eclipse-workspace\simpleOrdering\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D20174D-3A0B-4CC4-AB10-1843998852DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D060F899-3E0D-4204-9A30-50B30CCC8597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment_DirectSales" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
   <si>
     <t>Variable</t>
   </si>
@@ -206,6 +206,15 @@
   </si>
   <si>
     <t>Fix Voice Value Added Services</t>
+  </si>
+  <si>
+    <t>nonMobileVoice</t>
+  </si>
+  <si>
+    <t>optyStageCloseWon</t>
+  </si>
+  <si>
+    <t>Closed Won</t>
   </si>
 </sst>
 </file>
@@ -759,10 +768,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798AD516-E464-4708-9D8E-52009CD3236C}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,6 +890,22 @@
       </c>
       <c r="B14" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -961,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B66D6326-C1D0-467D-8F1E-D5B4A578621C}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
07/01 - MidDay Commit LA's
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.achas\eclipse-workspace\simpleOrdering\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D060F899-3E0D-4204-9A30-50B30CCC8597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB005BD-94E4-4444-8B41-CC6537828445}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
@@ -771,7 +771,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
08/01 - EOD Commit LA
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.achas\eclipse-workspace\simpleOrdering\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB005BD-94E4-4444-8B41-CC6537828445}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85E6A82-3191-42D1-B12B-596EDA255355}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="64">
   <si>
     <t>Variable</t>
   </si>
@@ -215,6 +215,18 @@
   </si>
   <si>
     <t>Closed Won</t>
+  </si>
+  <si>
+    <t>testingCompanySOI69</t>
+  </si>
+  <si>
+    <t>AutoTestingCompany_SOI69</t>
+  </si>
+  <si>
+    <t>idTestingCompanySOI69</t>
+  </si>
+  <si>
+    <t>0013E00000zXuBpQAK</t>
   </si>
 </sst>
 </file>
@@ -768,10 +780,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798AD516-E464-4708-9D8E-52009CD3236C}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,97 +826,113 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="3">
-        <v>5</v>
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="3">
-        <v>12</v>
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+      <c r="B13" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="B14" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>58</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
12/02 - New Branch commit
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.achas\eclipse-workspace\simpleOrdering\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85E6A82-3191-42D1-B12B-596EDA255355}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980E86FD-1708-4942-94F4-23F881FC84AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment_DirectSales" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
   <si>
     <t>Variable</t>
   </si>
@@ -58,9 +60,6 @@
     <t>envPasswordITTQA</t>
   </si>
   <si>
-    <t>Testing-2021</t>
-  </si>
-  <si>
     <t>homepage</t>
   </si>
   <si>
@@ -227,6 +226,39 @@
   </si>
   <si>
     <t>0013E00000zXuBpQAK</t>
+  </si>
+  <si>
+    <t>AutoTestingCompany_SOI79</t>
+  </si>
+  <si>
+    <t>testingCompanySOI79</t>
+  </si>
+  <si>
+    <t>idTestingCompanySOI79</t>
+  </si>
+  <si>
+    <t>0013E00000zZ4ccQAC</t>
+  </si>
+  <si>
+    <t>noServiceErrorMessage</t>
+  </si>
+  <si>
+    <t>This order can't be submited!No services associated to the order.</t>
+  </si>
+  <si>
+    <t>This order can't be submitted.One or more services without files</t>
+  </si>
+  <si>
+    <t>noFilesOnServiceErrorMessage</t>
+  </si>
+  <si>
+    <t>André Esteves</t>
+  </si>
+  <si>
+    <t>companyContactPerson</t>
+  </si>
+  <si>
+    <t>Testing-2022</t>
   </si>
 </sst>
 </file>
@@ -606,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +668,7 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -645,55 +677,55 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -702,6 +734,7 @@
     <hyperlink ref="B6" r:id="rId2" display="https://proximus--prxquodev.lightning.force.com/lightning/o/Account/new" xr:uid="{E8DAAB31-7462-4A23-B60C-1B00232CDC0B}"/>
     <hyperlink ref="B7" r:id="rId3" display="https://proximus--prxquodev.lightning.force.com/lightning/o/Account/list?filterName=Recent" xr:uid="{0D3112C4-7EFB-42A2-B310-867B69A1DDCB}"/>
     <hyperlink ref="B8" r:id="rId4" display="https://proximus--prxquodev.lightning.force.com/lightning/o/Opportunity/list?filterName=Recent" xr:uid="{6B1F7BAA-2D33-469A-A0D7-0501011B87BC}"/>
+    <hyperlink ref="B3" r:id="rId5" xr:uid="{3F3B749A-9973-4083-A2DE-12B0AD0D0DD8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -734,7 +767,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -742,7 +775,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -750,15 +783,15 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -780,10 +813,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798AD516-E464-4708-9D8E-52009CD3236C}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,138 +835,178 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
         <v>60</v>
-      </c>
-      <c r="B5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="3">
-        <v>5</v>
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="3">
-        <v>12</v>
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="B16" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
         <v>58</v>
       </c>
-      <c r="B18" t="s">
-        <v>59</v>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -966,42 +1039,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
         <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1034,42 +1107,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
         <v>55</v>
-      </c>
-      <c r="B2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20/02 - New Commit. New revision made: Report, sikuli and Steps.
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.achas\eclipse-workspace\simpleOrdering\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980E86FD-1708-4942-94F4-23F881FC84AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0239D1E-C5CD-4BC8-9645-F286597E66A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment_DirectSales" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="88">
   <si>
     <t>Variable</t>
   </si>
@@ -48,9 +48,6 @@
     <t>environmentITTQA</t>
   </si>
   <si>
-    <t>https://test.salesforce.com</t>
-  </si>
-  <si>
     <t>envUserNameITTQA</t>
   </si>
   <si>
@@ -259,6 +256,51 @@
   </si>
   <si>
     <t>Testing-2022</t>
+  </si>
+  <si>
+    <t>testingCompanySOI150</t>
+  </si>
+  <si>
+    <t>AutoTestingCompany_SOI150</t>
+  </si>
+  <si>
+    <t>idTestingCompanySOI150</t>
+  </si>
+  <si>
+    <t>0013E00001A00FRQAZ</t>
+  </si>
+  <si>
+    <t>testingCompanySOI76</t>
+  </si>
+  <si>
+    <t>AutoTestingCompany_SOI76</t>
+  </si>
+  <si>
+    <t>idTestingCompanySOI76</t>
+  </si>
+  <si>
+    <t>0013E00001A0KOSQA3</t>
+  </si>
+  <si>
+    <t>envUsernameNameITTQA</t>
+  </si>
+  <si>
+    <t>Miguel Gonçalves</t>
+  </si>
+  <si>
+    <t>envUserProfileITTQA</t>
+  </si>
+  <si>
+    <t>PRX_Sales User Profile</t>
+  </si>
+  <si>
+    <t>https://proximusitqa--prxittqa.lightning.force.com</t>
+  </si>
+  <si>
+    <t>newOpportunityLink</t>
+  </si>
+  <si>
+    <t>https://proximusitqa--prxittqa.lightning.force.com/lightning/o/Opportunity/new?count=2&amp;nooverride=1&amp;useRecordTypeCheck=1&amp;navigationLocation=LIST_VIEW&amp;backgroundContext=%2Flightning%2Fr%2FContact%2F0033E00001COoP2QAL%2Fview</t>
   </si>
 </sst>
 </file>
@@ -636,15 +678,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="90" customWidth="1"/>
   </cols>
   <sheetData>
@@ -660,81 +702,107 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="B2" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
-        <v>27</v>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="https://proximus--prxquodev.lightning.force.com/lightning/page/home" xr:uid="{97A41C80-C6B4-42A3-B3D0-DFB1FE93C23A}"/>
-    <hyperlink ref="B6" r:id="rId2" display="https://proximus--prxquodev.lightning.force.com/lightning/o/Account/new" xr:uid="{E8DAAB31-7462-4A23-B60C-1B00232CDC0B}"/>
-    <hyperlink ref="B7" r:id="rId3" display="https://proximus--prxquodev.lightning.force.com/lightning/o/Account/list?filterName=Recent" xr:uid="{0D3112C4-7EFB-42A2-B310-867B69A1DDCB}"/>
-    <hyperlink ref="B8" r:id="rId4" display="https://proximus--prxquodev.lightning.force.com/lightning/o/Opportunity/list?filterName=Recent" xr:uid="{6B1F7BAA-2D33-469A-A0D7-0501011B87BC}"/>
+    <hyperlink ref="B7" r:id="rId1" display="https://proximus--prxquodev.lightning.force.com/lightning/page/home" xr:uid="{97A41C80-C6B4-42A3-B3D0-DFB1FE93C23A}"/>
+    <hyperlink ref="B8" r:id="rId2" display="https://proximus--prxquodev.lightning.force.com/lightning/o/Account/new" xr:uid="{E8DAAB31-7462-4A23-B60C-1B00232CDC0B}"/>
+    <hyperlink ref="B9" r:id="rId3" display="https://proximus--prxquodev.lightning.force.com/lightning/o/Account/list?filterName=Recent" xr:uid="{0D3112C4-7EFB-42A2-B310-867B69A1DDCB}"/>
+    <hyperlink ref="B10" r:id="rId4" display="https://proximus--prxquodev.lightning.force.com/lightning/o/Opportunity/list?filterName=Recent" xr:uid="{6B1F7BAA-2D33-469A-A0D7-0501011B87BC}"/>
     <hyperlink ref="B3" r:id="rId5" xr:uid="{3F3B749A-9973-4083-A2DE-12B0AD0D0DD8}"/>
+    <hyperlink ref="B2" r:id="rId6" xr:uid="{FAEE0540-D280-463B-A7A4-16B691FBE90F}"/>
+    <hyperlink ref="B13" r:id="rId7" xr:uid="{90510573-C6CD-4BBF-84B6-CE0CDC82ACFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -767,31 +835,31 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -813,10 +881,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798AD516-E464-4708-9D8E-52009CD3236C}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,178 +903,210 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
         <v>59</v>
-      </c>
-      <c r="B5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
         <v>48</v>
-      </c>
-      <c r="B9" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="3">
-        <v>5</v>
+        <v>75</v>
+      </c>
+      <c r="B15" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="3">
-        <v>12</v>
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" t="s">
-        <v>55</v>
+        <v>33</v>
+      </c>
+      <c r="B19" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" t="s">
-        <v>58</v>
+        <v>34</v>
+      </c>
+      <c r="B20" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1039,42 +1139,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1107,42 +1207,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
         <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
27/02 - SOI-770 & SOI-720
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.achas\eclipse-workspace\simpleOrdering\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367DE8D8-E2C6-4884-BB46-4C9F93A3501D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE26A1B1-1536-441C-8930-A6411628F8E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment_DirectSales" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="110">
   <si>
     <t>Variable</t>
   </si>
@@ -343,6 +343,30 @@
   </si>
   <si>
     <t>/lightning/o/csord__Order__c/home</t>
+  </si>
+  <si>
+    <t>testingCompanySOI720</t>
+  </si>
+  <si>
+    <t>testingCompanySOI770</t>
+  </si>
+  <si>
+    <t>AutoTestingCompany_SOI720</t>
+  </si>
+  <si>
+    <t>AutoTestingCompany_SOI770</t>
+  </si>
+  <si>
+    <t>0013E00001AAevfQAD</t>
+  </si>
+  <si>
+    <t>idTestingCompanySOI720</t>
+  </si>
+  <si>
+    <t>idTestingCompanySOI770</t>
+  </si>
+  <si>
+    <t>0013E00001AAevVQAT</t>
   </si>
 </sst>
 </file>
@@ -722,7 +746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -931,10 +955,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798AD516-E464-4708-9D8E-52009CD3236C}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,177 +1057,209 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>102</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="3">
-        <v>5</v>
+        <v>108</v>
+      </c>
+      <c r="B25" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="3">
-        <v>12</v>
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" t="s">
-        <v>54</v>
+        <v>33</v>
+      </c>
+      <c r="B29" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" t="s">
-        <v>57</v>
+        <v>34</v>
+      </c>
+      <c r="B30" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>71</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B37" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
02/03 - SOI-721: TC1+TC3
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.achas\eclipse-workspace\simpleOrdering\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE26A1B1-1536-441C-8930-A6411628F8E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D13CC46-6153-487E-9770-54F7AADB6B27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment_DirectSales" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="114">
   <si>
     <t>Variable</t>
   </si>
@@ -367,13 +367,25 @@
   </si>
   <si>
     <t>0013E00001AAevVQAT</t>
+  </si>
+  <si>
+    <t>testingCompanySOI721</t>
+  </si>
+  <si>
+    <t>AutoTestingCompany_SOI721</t>
+  </si>
+  <si>
+    <t>idTestingCompanySOI721</t>
+  </si>
+  <si>
+    <t>0013E00001AB2CVQA1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,6 +405,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -955,10 +973,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798AD516-E464-4708-9D8E-52009CD3236C}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,205 +1083,222 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="B24" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B25" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>112</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="3">
-        <v>5</v>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="3">
-        <v>12</v>
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="B31" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="B32" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>71</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
09/03 - First commit of the day
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.achas\eclipse-workspace\simpleOrdering\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2718BF-FB57-4BA8-A7FE-55B1CF5AF179}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA9229F-B3A1-48E2-B653-6003EECC767A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment_DirectSales" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="122">
   <si>
     <t>Variable</t>
   </si>
@@ -391,6 +391,18 @@
   </si>
   <si>
     <t>0013E00001ABMzEQAX</t>
+  </si>
+  <si>
+    <t>testingCompanySOI880</t>
+  </si>
+  <si>
+    <t>AutoTestingCompany_SOI880</t>
+  </si>
+  <si>
+    <t>idTestingCompanySOI880</t>
+  </si>
+  <si>
+    <t>0013E00001ABencQAD</t>
   </si>
 </sst>
 </file>
@@ -985,10 +997,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798AD516-E464-4708-9D8E-52009CD3236C}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,217 +1123,233 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B26" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B29" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>116</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="3">
-        <v>5</v>
+        <v>27</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="3">
-        <v>12</v>
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="B35" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="B36" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>70</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
13/03 - EOD Commit
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.achas\eclipse-workspace\simpleOrdering\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA9229F-B3A1-48E2-B653-6003EECC767A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E17954B-C614-469C-877E-C38C40334880}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment_DirectSales" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="133">
   <si>
     <t>Variable</t>
   </si>
@@ -403,6 +403,39 @@
   </si>
   <si>
     <t>0013E00001ABencQAD</t>
+  </si>
+  <si>
+    <t>approverProfileUser</t>
+  </si>
+  <si>
+    <t>approverProfilePass</t>
+  </si>
+  <si>
+    <t>costumerSupportProfileUser</t>
+  </si>
+  <si>
+    <t>costumerSupportProfilePass</t>
+  </si>
+  <si>
+    <t>salesSupportProfileUser</t>
+  </si>
+  <si>
+    <t>salesSupportProfilePass</t>
+  </si>
+  <si>
+    <t>andre.esteves.ext@proximus.com.aprv</t>
+  </si>
+  <si>
+    <t>Inno6677!</t>
+  </si>
+  <si>
+    <t>andre.esteves.ext@proximus.com.csupp</t>
+  </si>
+  <si>
+    <t>andre.esteves.ext@proximus.com.ssupp</t>
+  </si>
+  <si>
+    <t>Win6677!</t>
   </si>
 </sst>
 </file>
@@ -786,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,6 +941,54 @@
       </c>
       <c r="B14" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>127</v>
+      </c>
+      <c r="B20" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -999,7 +1080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798AD516-E464-4708-9D8E-52009CD3236C}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
14/07 - Commit EOD
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.achas\eclipse-workspace\simpleOrdering\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E66F5B3-55B6-484A-8231-61FA326286B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD7BAFC-5AFF-4371-82A0-2A1F0B77028B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment_DirectSales" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="137">
   <si>
     <t>Variable</t>
   </si>
@@ -436,6 +436,18 @@
   </si>
   <si>
     <t>Testing-2023</t>
+  </si>
+  <si>
+    <t>testingCompanySOI1312</t>
+  </si>
+  <si>
+    <t>AutoTestingCompany_SOI1312</t>
+  </si>
+  <si>
+    <t>0013E00001CtYgQQAV</t>
+  </si>
+  <si>
+    <t>idTestingCompanySOI1312</t>
   </si>
 </sst>
 </file>
@@ -821,7 +833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1078,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798AD516-E464-4708-9D8E-52009CD3236C}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,225 +1224,241 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B29" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B30" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="B31" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>114</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="3">
-        <v>5</v>
+        <v>27</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="3">
-        <v>12</v>
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>34</v>
-      </c>
-      <c r="B37" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="B37" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="B38" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B42" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>70</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B45" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
17/08 - TestData File
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.achas\eclipse-workspace\simpleOrdering\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntake\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D83B6C-A7B6-48B1-9183-E39A63FD46EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69840EB5-BBCC-4890-BADB-43C48B2A80F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment_DirectSales" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="179">
   <si>
     <t>Variable</t>
   </si>
@@ -566,6 +566,9 @@
   </si>
   <si>
     <t>webFormPass</t>
+  </si>
+  <si>
+    <t>Testing Sales User</t>
   </si>
 </sst>
 </file>
@@ -960,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,6 +1008,9 @@
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1148,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5665C1EA-CD7B-46F0-96D7-3CD986315FA1}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
27/08 - Code Review Meeting - 1st
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntake\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69840EB5-BBCC-4890-BADB-43C48B2A80F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EBA7CD-5E47-463B-AC98-F273F7FF3512}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment_DirectSales" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="180">
   <si>
     <t>Variable</t>
   </si>
@@ -569,6 +569,9 @@
   </si>
   <si>
     <t>Testing Sales User</t>
+  </si>
+  <si>
+    <t>SOI Testing Farmer</t>
   </si>
 </sst>
 </file>
@@ -963,7 +966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -1152,15 +1155,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5665C1EA-CD7B-46F0-96D7-3CD986315FA1}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="90" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1198,73 +1201,81 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>132</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" t="s">
-        <v>123</v>
+        <v>129</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
+      </c>
+      <c r="B8" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B9" t="s">
-        <v>123</v>
+        <v>128</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>175</v>
+        <v>136</v>
       </c>
       <c r="B11" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>175</v>
+      </c>
+      <c r="B12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>177</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>123</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{E8C1F140-AA4E-47FA-B7B1-FF578BEB2CB8}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{90668D52-F773-4721-8F55-5CE4B002CE0F}"/>
-    <hyperlink ref="B8" r:id="rId3" xr:uid="{09E8ECF8-60A5-4BC1-9D91-44A94507D548}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{90668D52-F773-4721-8F55-5CE4B002CE0F}"/>
+    <hyperlink ref="B9" r:id="rId3" xr:uid="{09E8ECF8-60A5-4BC1-9D91-44A94507D548}"/>
     <hyperlink ref="B2" r:id="rId4" xr:uid="{17BFAB06-CF1A-49F3-AC65-E4C130025861}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>